<commit_message>
Export vers database focntionne. Modification du nom de ficher pour t_projet import Ajout de la fonction pandas
</commit_message>
<xml_diff>
--- a/API/Crypto.xlsx
+++ b/API/Crypto.xlsx
@@ -1,33 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidbolduc/PycharmProjects/GIT_DEPOT_GLO-2005/API/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gohab\PycharmProjects\GIT_DEPOT_GLO-2005\API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A56097A-21AC-BC43-9999-56735330BFC3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91129893-7BCF-4DBD-9114-791942CB7048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="780" yWindow="500" windowWidth="25100" windowHeight="20500" xr2:uid="{673F19DF-2096-D34F-8D4D-F7C3B1A47F48}"/>
+    <workbookView xWindow="38805" yWindow="2070" windowWidth="28800" windowHeight="15435" xr2:uid="{673F19DF-2096-D34F-8D4D-F7C3B1A47F48}"/>
   </bookViews>
   <sheets>
     <sheet name="t_projet" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -231,63 +222,6 @@
     <t>Coin Coin</t>
   </si>
   <si>
-    <t>2013-04-28T00:00:00</t>
-  </si>
-  <si>
-    <t>2015-08-07T00:00:00</t>
-  </si>
-  <si>
-    <t>2017-07-25T00:00:00</t>
-  </si>
-  <si>
-    <t>2013-08-04T00:00:00</t>
-  </si>
-  <si>
-    <t>2015-02-25T00:00:00</t>
-  </si>
-  <si>
-    <t>2013-12-15T00:00:00</t>
-  </si>
-  <si>
-    <t>2017-10-01T00:00:00</t>
-  </si>
-  <si>
-    <t>2020-08-19T00:00:00</t>
-  </si>
-  <si>
-    <t>2020-09-17T00:00:00</t>
-  </si>
-  <si>
-    <t>2017-07-23T00:00:00</t>
-  </si>
-  <si>
-    <t>2017-09-20T00:00:00</t>
-  </si>
-  <si>
-    <t>2018-10-08T00:00:00</t>
-  </si>
-  <si>
-    <t>2017-08-22T00:00:00</t>
-  </si>
-  <si>
-    <t>2020-04-10T00:00:00</t>
-  </si>
-  <si>
-    <t>2014-08-05T00:00:00</t>
-  </si>
-  <si>
-    <t>2017-12-13T00:00:00</t>
-  </si>
-  <si>
-    <t>2018-01-17T00:00:00</t>
-  </si>
-  <si>
-    <t>2017-09-13T00:00:00</t>
-  </si>
-  <si>
-    <t>2019-01-30T00:00:00</t>
-  </si>
-  <si>
     <t>Prix actuel</t>
   </si>
   <si>
@@ -310,6 +244,63 @@
   </si>
   <si>
     <t>Qte Circulation</t>
+  </si>
+  <si>
+    <t>2013-04-28</t>
+  </si>
+  <si>
+    <t>2015-08-07</t>
+  </si>
+  <si>
+    <t>2017-07-25</t>
+  </si>
+  <si>
+    <t>2013-08-04</t>
+  </si>
+  <si>
+    <t>2015-02-25</t>
+  </si>
+  <si>
+    <t>2013-12-15</t>
+  </si>
+  <si>
+    <t>2017-10-01</t>
+  </si>
+  <si>
+    <t>2020-08-19</t>
+  </si>
+  <si>
+    <t>2020-09-17</t>
+  </si>
+  <si>
+    <t>2017-07-23</t>
+  </si>
+  <si>
+    <t>2017-09-20</t>
+  </si>
+  <si>
+    <t>2018-10-08</t>
+  </si>
+  <si>
+    <t>2017-08-22</t>
+  </si>
+  <si>
+    <t>2020-04-10</t>
+  </si>
+  <si>
+    <t>2014-08-05</t>
+  </si>
+  <si>
+    <t>2017-12-13</t>
+  </si>
+  <si>
+    <t>2018-01-17</t>
+  </si>
+  <si>
+    <t>2017-09-13</t>
+  </si>
+  <si>
+    <t>2019-01-30</t>
   </si>
 </sst>
 </file>
@@ -797,21 +788,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E590085-84D7-CF49-B7D2-21B8B45744FC}">
-  <dimension ref="A1:X28"/>
+  <dimension ref="A1:W28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F21"/>
+      <selection activeCell="E2" sqref="E2:E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="38.1640625" customWidth="1"/>
+    <col min="2" max="2" width="38.125" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="14" max="14" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -830,32 +821,32 @@
       <c r="F1" t="s">
         <v>57</v>
       </c>
+      <c r="G1" t="s">
+        <v>65</v>
+      </c>
       <c r="H1" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="I1" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="J1" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="K1" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="L1" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="M1" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="N1" t="s">
-        <v>91</v>
-      </c>
-      <c r="O1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -869,7 +860,7 @@
         <v>64</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="F2" s="4">
         <v>1</v>
@@ -891,9 +882,8 @@
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
       <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -907,13 +897,13 @@
         <v>64</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="F3" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -927,13 +917,13 @@
         <v>64</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="F4" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -947,13 +937,13 @@
         <v>64</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="F5" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -967,13 +957,13 @@
         <v>64</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="F6" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -987,13 +977,13 @@
         <v>64</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="F7" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1007,13 +997,13 @@
         <v>64</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="F8" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1027,13 +1017,13 @@
         <v>64</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="F9" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1047,13 +1037,13 @@
         <v>64</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="F10" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1067,13 +1057,13 @@
         <v>64</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F11" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1087,13 +1077,13 @@
         <v>64</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="F12" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -1107,13 +1097,13 @@
         <v>64</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="F13" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>55</v>
       </c>
@@ -1127,13 +1117,13 @@
         <v>64</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="F14" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1147,13 +1137,13 @@
         <v>64</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="F15" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1167,13 +1157,13 @@
         <v>64</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="F16" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -1187,13 +1177,13 @@
         <v>64</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="F17" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -1207,13 +1197,13 @@
         <v>64</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="F18" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1227,13 +1217,13 @@
         <v>64</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="F19" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -1247,13 +1237,13 @@
         <v>64</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="F20" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -1267,34 +1257,34 @@
         <v>64</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="F21" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E22" s="2"/>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
-      <c r="F25" s="2"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
     </row>
   </sheetData>
@@ -1321,5 +1311,6 @@
     <hyperlink ref="B21" r:id="rId20" xr:uid="{D4297ADE-6F8F-D447-9FE4-6F68ACBE5133}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>